<commit_message>
updated role and user
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/01-BulkUploadRole.xlsx
+++ b/documents/templates/bulk-upload/01-BulkUploadRole.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B651848F-D652-6943-B446-57C060620F39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC0C1BD-4284-6E40-A855-6004C971A56A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>Logistics</t>
   </si>
   <si>
-    <t>Engineering</t>
-  </si>
-  <si>
     <t>Production</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Store</t>
+  </si>
+  <si>
+    <t>Process</t>
   </si>
 </sst>
 </file>
@@ -67,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,12 +75,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,7 +380,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -393,23 +409,23 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>